<commit_message>
add sort -val and -data  func
</commit_message>
<xml_diff>
--- a/Analyze_file.xlsx
+++ b/Analyze_file.xlsx
@@ -354,7 +354,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -380,50 +380,80 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>خوراکی</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>30000</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1400/01/01</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Allocation</t>
+          <t>خوراکی</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>200000</v>
+        <v>10000</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>***</t>
+          <t>1400/01/10</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Expend</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>***</t>
-        </is>
-      </c>
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Remaining</t>
+          <t>Allocation</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>200000</v>
       </c>
       <c r="C5" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Expend</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>40000</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Remaining</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>160000</v>
+      </c>
+      <c r="C7" t="inlineStr">
         <is>
           <t>***</t>
         </is>
@@ -480,10 +510,10 @@
         <v>200000</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="D2" t="n">
-        <v>200000</v>
+        <v>160000</v>
       </c>
     </row>
     <row r="3">
@@ -630,10 +660,10 @@
         <v>2500000</v>
       </c>
       <c r="C12" t="n">
-        <v>2000000</v>
+        <v>2040000</v>
       </c>
       <c r="D12" t="n">
-        <v>500000</v>
+        <v>460000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>